<commit_message>
Implemented Verification methods for Registration process
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fordprefect/Documents/Weiterbildungen/Test Automation Engineer/II Selenium 3.0 Training/AutomationProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36067B0A-5FDC-4648-921B-D1248331B64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F59561-786B-0540-A33A-A06F98AE4967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{2B2F0D9C-3928-4146-9767-58840915A127}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Ford</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>New York</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, consetetur sadipscing elitr, sed diam nonumy eirmod tempor invidunt ut labore et dolore magna aliquyam</t>
   </si>
   <si>
@@ -146,7 +140,31 @@
     <t>Adress2</t>
   </si>
   <si>
-    <t>Indiana</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>01234567890</t>
+  </si>
+  <si>
+    <t>01787965432</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>aab@aab.com</t>
+  </si>
+  <si>
+    <t>aabtest1@aab.com</t>
   </si>
 </sst>
 </file>
@@ -510,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E717921-FADA-E947-A707-246503B2DDF4}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,49 +565,49 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
       <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -612,60 +630,204 @@
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1">
         <v>1983</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="O2" s="1">
         <v>48</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1983</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="1">
+        <v>48</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="1">
-        <v>1234</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="T3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
         <v>31</v>
       </c>
-      <c r="U2" s="1">
-        <v>1234567890</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1787965432</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>32</v>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1983</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="1">
+        <v>48</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{37196E11-81F8-2445-B46F-D9767036300C}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{7EC7B737-34B8-6343-8D04-6B7F62575D05}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{2F3B5E98-991F-0549-8C54-07A6FF2B6AD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>